<commit_message>
added above 10 books script
</commit_message>
<xml_diff>
--- a/Tests/Data/Account_Numbers.xlsx
+++ b/Tests/Data/Account_Numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ganesh/Postal-Automation/Tests/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FCFF58-A7A8-844C-A728-0B4456EB2D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F525AD9D-BEA2-1345-9000-9531D6C4A1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{6D22EA5D-F275-164D-90D9-4805AC948F77}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="397">
   <si>
     <t>Account Number</t>
   </si>
@@ -1224,7 +1224,10 @@
     <t>4951947865</t>
   </si>
   <si>
-    <t>4951824081,4769960896,4733733532,020092433488,020085461647,020069752419,9451335644,5005414487,4846262240,4951947865</t>
+    <t>4663597082</t>
+  </si>
+  <si>
+    <t>4951824081,4769960896,4733733532,020092433488,020085461647,020069752419,9451335644,5005414487,4846262240,4951947865,020000056862,4663597082</t>
   </si>
 </sst>
 </file>
@@ -1644,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F0B4C5-713C-6140-9AFF-43D389104A0A}">
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView topLeftCell="A217" zoomScale="170" workbookViewId="0">
-      <selection activeCell="B232" sqref="B232"/>
+    <sheetView topLeftCell="A179" zoomScale="170" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5725,8 +5728,8 @@
       <c r="A198" s="3">
         <v>197</v>
       </c>
-      <c r="B198" s="12">
-        <v>4663597082</v>
+      <c r="B198" s="12" t="s">
+        <v>395</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>194</v>
@@ -6634,9 +6637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9700EE86-16C6-6E45-B020-2AE7AE0924A2}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6645,7 +6646,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="46" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>